<commit_message>
add most of presentation graphs
</commit_message>
<xml_diff>
--- a/results/graphs/us-east-graphs.xlsx
+++ b/results/graphs/us-east-graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Google Drive/serverlessComputingProject/7x24/results/graphs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E5CF7A-0333-D743-B2FA-506F041B950A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98AD8E3D-E409-514A-8987-D163D6CC9BE5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{215248B2-6CD5-D841-804D-71CAA8927BE0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="17920" windowHeight="21900" xr2:uid="{215248B2-6CD5-D841-804D-71CAA8927BE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -118,11 +122,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>US-East-1</a:t>
+              <a:t>US-East-2</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> 128MB</a:t>
+              <a:t> 2048MB</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -155,7 +159,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="8">
-                  <c:v>360</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -163,37 +167,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-3895-4641-8BAA-1E108F44FE1C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$G$1:$G$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="8">
-                  <c:v>360</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-3895-4641-8BAA-1E108F44FE1C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -237,7 +210,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Coldstarts</a:t>
+                  <a:t>Warmstarts</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -336,7 +309,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Seconds until Coldstart</a:t>
+                  <a:t>Seconds until Warmstart</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -510,7 +483,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="8">
-                  <c:v>360</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -561,7 +534,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Coldstarts</a:t>
+                  <a:t>Warmstarts</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -680,7 +653,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Seconds until Coldstart</a:t>
+                  <a:t>Seconds until Warmstart</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -902,7 +875,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="8">
-                  <c:v>360</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1294,7 +1267,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="8">
-                  <c:v>360</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1345,7 +1318,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Coldstarts</a:t>
+                  <a:t>Warmstarts</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1464,7 +1437,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Seconds until Coldstart</a:t>
+                  <a:t>Seconds until Warmstart</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1657,7 +1630,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="8">
-                  <c:v>360</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1665,37 +1638,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-BDC0-A14D-B472-8B418D733387}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$G$1:$G$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="8">
-                  <c:v>360</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-BDC0-A14D-B472-8B418D733387}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2012,7 +1954,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="8">
-                  <c:v>360</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2404,7 +2346,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="8">
-                  <c:v>360</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2796,7 +2738,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="8">
-                  <c:v>360</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6946,7 +6888,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6970,16 +6912,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>360</v>
+        <v>420</v>
       </c>
       <c r="B2">
-        <v>360</v>
+        <v>420</v>
       </c>
       <c r="C2">
-        <v>360</v>
+        <v>420</v>
       </c>
       <c r="D2">
-        <v>360</v>
+        <v>420</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -6996,11 +6938,29 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>360</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
       <c r="F5">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>360</v>
+      </c>
+      <c r="C6">
+        <v>300</v>
+      </c>
+      <c r="D6">
+        <v>300</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
       <c r="F6">
         <v>6</v>
       </c>
@@ -7020,7 +6980,7 @@
         <v>9</v>
       </c>
       <c r="G9">
-        <v>360</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>